<commit_message>
update genet names for merging with 2020 data, and fix error (ML71 should have been ML77 based on field notes)
</commit_message>
<xml_diff>
--- a/data/reproducibility/genet_map.xlsx
+++ b/data/reproducibility/genet_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcunning/Projects/CBASS_methods/data/reproducibility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B892EEA1-A6B1-5843-B6CF-D80F926E47FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0800DF-A6D0-F84B-86C5-AE946BD4865C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29780" yWindow="2520" windowWidth="27640" windowHeight="16440" xr2:uid="{C65CA909-C6F2-E443-91D0-CA458C64F66D}"/>
+    <workbookView xWindow="-29780" yWindow="1560" windowWidth="27640" windowHeight="16440" xr2:uid="{C65CA909-C6F2-E443-91D0-CA458C64F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -177,9 +177,6 @@
     <t>ML47</t>
   </si>
   <si>
-    <t>ML71</t>
-  </si>
-  <si>
     <t>ML41</t>
   </si>
   <si>
@@ -291,18 +288,9 @@
     <t>CRF055</t>
   </si>
   <si>
-    <t>Acer121</t>
-  </si>
-  <si>
-    <t>Acer120</t>
-  </si>
-  <si>
     <t>CRF087</t>
   </si>
   <si>
-    <t>Acer123</t>
-  </si>
-  <si>
     <t>CRF024</t>
   </si>
   <si>
@@ -310,6 +298,18 @@
   </si>
   <si>
     <t>55y</t>
+  </si>
+  <si>
+    <t>Acer121RR</t>
+  </si>
+  <si>
+    <t>Acer120RR</t>
+  </si>
+  <si>
+    <t>Acer123RR</t>
+  </si>
+  <si>
+    <t>ML77</t>
   </si>
 </sst>
 </file>
@@ -372,7 +372,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -660,7 +660,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -670,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE9305B-3BE8-834C-8C49-186205CFF357}">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -693,12 +693,12 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -710,12 +710,12 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -727,12 +727,12 @@
         <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -744,12 +744,12 @@
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -761,12 +761,12 @@
         <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
@@ -778,12 +778,12 @@
         <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
@@ -795,12 +795,12 @@
         <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
@@ -812,12 +812,12 @@
         <v>21</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>11</v>
@@ -829,12 +829,12 @@
         <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
@@ -846,12 +846,12 @@
         <v>23</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
@@ -863,12 +863,12 @@
         <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>12</v>
@@ -880,12 +880,12 @@
         <v>25</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
@@ -897,12 +897,12 @@
         <v>26</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
@@ -914,12 +914,12 @@
         <v>27</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>12</v>
@@ -931,12 +931,12 @@
         <v>28</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>12</v>
@@ -948,12 +948,12 @@
         <v>29</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
@@ -965,12 +965,12 @@
         <v>30</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
@@ -982,12 +982,12 @@
         <v>31</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>13</v>
@@ -999,12 +999,12 @@
         <v>32</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
@@ -1016,12 +1016,12 @@
         <v>33</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>13</v>
@@ -1033,12 +1033,12 @@
         <v>34</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>14</v>
@@ -1050,12 +1050,12 @@
         <v>35</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>14</v>
@@ -1064,15 +1064,15 @@
         <v>7</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>14</v>
@@ -1084,12 +1084,12 @@
         <v>36</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>14</v>
@@ -1101,12 +1101,12 @@
         <v>37</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>14</v>
@@ -1115,15 +1115,15 @@
         <v>10</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>15</v>
@@ -1135,12 +1135,12 @@
         <v>38</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>15</v>
@@ -1152,12 +1152,12 @@
         <v>39</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>15</v>
@@ -1169,12 +1169,12 @@
         <v>40</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>3</v>
@@ -1183,15 +1183,15 @@
         <v>4</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>3</v>
@@ -1203,12 +1203,12 @@
         <v>44</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>3</v>
@@ -1220,12 +1220,12 @@
         <v>45</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>3</v>
@@ -1234,15 +1234,15 @@
         <v>9</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>3</v>
@@ -1254,12 +1254,12 @@
         <v>46</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>3</v>
@@ -1268,15 +1268,15 @@
         <v>41</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>3</v>
@@ -1285,15 +1285,15 @@
         <v>42</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>3</v>
@@ -1302,15 +1302,15 @@
         <v>43</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>11</v>
@@ -1319,15 +1319,15 @@
         <v>4</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>11</v>
@@ -1336,15 +1336,15 @@
         <v>7</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>11</v>
@@ -1353,15 +1353,15 @@
         <v>8</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>11</v>
@@ -1370,15 +1370,15 @@
         <v>9</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>11</v>
@@ -1387,15 +1387,15 @@
         <v>10</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>11</v>
@@ -1404,15 +1404,15 @@
         <v>41</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>11</v>
@@ -1421,15 +1421,15 @@
         <v>42</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>11</v>
@@ -1438,15 +1438,15 @@
         <v>43</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>13</v>
@@ -1455,15 +1455,15 @@
         <v>4</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>13</v>
@@ -1472,15 +1472,15 @@
         <v>7</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>13</v>
@@ -1489,15 +1489,15 @@
         <v>8</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>13</v>
@@ -1506,15 +1506,15 @@
         <v>9</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>13</v>
@@ -1523,15 +1523,15 @@
         <v>10</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>13</v>
@@ -1540,15 +1540,15 @@
         <v>41</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>13</v>
@@ -1557,15 +1557,15 @@
         <v>42</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>13</v>
@@ -1574,15 +1574,15 @@
         <v>43</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>12</v>
@@ -1591,15 +1591,15 @@
         <v>4</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>12</v>
@@ -1608,15 +1608,15 @@
         <v>7</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>12</v>
@@ -1625,15 +1625,15 @@
         <v>8</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>12</v>
@@ -1642,15 +1642,15 @@
         <v>9</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>12</v>
@@ -1659,15 +1659,15 @@
         <v>10</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>12</v>
@@ -1676,15 +1676,15 @@
         <v>41</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>12</v>
@@ -1693,15 +1693,15 @@
         <v>42</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>12</v>
@@ -1710,15 +1710,15 @@
         <v>43</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>14</v>
@@ -1727,15 +1727,15 @@
         <v>4</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>14</v>
@@ -1744,15 +1744,15 @@
         <v>7</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>14</v>
@@ -1761,15 +1761,15 @@
         <v>8</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>14</v>
@@ -1778,15 +1778,15 @@
         <v>9</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>14</v>
@@ -1795,15 +1795,15 @@
         <v>10</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>14</v>
@@ -1812,15 +1812,15 @@
         <v>41</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>14</v>
@@ -1829,10 +1829,10 @@
         <v>42</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>